<commit_message>
Add more needed functions
</commit_message>
<xml_diff>
--- a/Incompatible Programs.xlsx
+++ b/Incompatible Programs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Programa</t>
   </si>
@@ -127,6 +127,21 @@
   </si>
   <si>
     <t>Ultra Compare</t>
+  </si>
+  <si>
+    <t>Git 2.9+</t>
+  </si>
+  <si>
+    <t>Em progresso</t>
+  </si>
+  <si>
+    <t>Git Hub</t>
+  </si>
+  <si>
+    <t>Atom</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
   </si>
 </sst>
 </file>
@@ -473,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -697,7 +712,7 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -721,6 +736,30 @@
         <v>36</v>
       </c>
       <c r="B29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>